<commit_message>
Fixed not sending proper rating
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nickl\Documents\GitHub\IsItToS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19C3D0D-9308-4CEE-B7C7-B88ACAA041F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="570" windowWidth="28455" windowHeight="11955"/>
+    <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -81,8 +87,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -119,6 +125,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -165,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -197,9 +211,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -231,6 +263,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -406,20 +456,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D10" sqref="A10:D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="55.25" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75">
+    <row r="1" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +479,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75">
+    <row r="2" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -447,7 +493,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -461,7 +507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75">
+    <row r="4" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -472,7 +518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75">
+    <row r="5" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -483,7 +529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75">
+    <row r="6" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -497,7 +543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75">
+    <row r="7" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -508,7 +554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75">
+    <row r="8" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -522,7 +568,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75">
+    <row r="9" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -536,6 +582,7 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:4" ht="15.6" x14ac:dyDescent="0.3"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -545,12 +592,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
@@ -560,12 +607,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/TeamAlt-F4/IsItToS"
This reverts commit 801ceb65c9657b9def147b2e966976cc074e417c, reversing
changes made to ecd0a1a10cbea5840d023ca510ccda958b0b4f74.
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -409,10 +409,10 @@
         <v>video_id</v>
       </c>
       <c r="B1" t="str">
-        <v>commentz</v>
+        <v>comments</v>
       </c>
       <c r="C1" t="str">
-        <v>moderatorRating</v>
+        <v>moderator_rating</v>
       </c>
       <c r="D1" t="str">
         <v>age_restricted</v>
@@ -521,24 +521,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v>7yzImCTv7A0</v>
-      </c>
-      <c r="B10" t="str">
-        <v/>
-      </c>
-      <c r="C10" t="str">
-        <v>safe</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D9"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>